<commit_message>
Corrigindo para apenas deputados federais de 2018
</commit_message>
<xml_diff>
--- a/2014/relatorioBR.xlsx
+++ b/2014/relatorioBR.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Foto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>SQ_CANDIDATO</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Código da Cor</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Cor</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Teve dificuldade para classificar?</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Houve erro na exibição da foto</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>UF</t>
         </is>
@@ -494,28 +499,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000062</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>62</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -535,20 +545,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000081</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>81</v>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -557,6 +567,11 @@
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -576,20 +591,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000065</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>65</v>
       </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F4" t="n">
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -598,6 +613,11 @@
         </is>
       </c>
       <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -617,20 +637,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000021</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>21</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F5" t="n">
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -639,6 +659,11 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -658,20 +683,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000084</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>84</v>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F6" t="n">
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -680,6 +705,11 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -699,20 +729,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000086</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>86</v>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F7" t="n">
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -721,6 +751,11 @@
         </is>
       </c>
       <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -740,20 +775,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000066</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>66</v>
       </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F8" t="n">
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -762,6 +797,11 @@
         </is>
       </c>
       <c r="I8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -781,20 +821,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000061</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>61</v>
       </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F9" t="n">
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -803,6 +843,11 @@
         </is>
       </c>
       <c r="I9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -822,20 +867,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000068</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>68</v>
       </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F10" t="n">
+        <v>1</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -844,6 +889,11 @@
         </is>
       </c>
       <c r="I10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -863,28 +913,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000002</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>2</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>3</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t xml:space="preserve"> Pardo / “Moreno” / Brown</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -904,20 +959,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000063</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>63</v>
       </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F12" t="n">
+        <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -926,6 +981,11 @@
         </is>
       </c>
       <c r="I12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -945,20 +1005,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000123</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>123</v>
       </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F13" t="n">
+        <v>1</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -967,6 +1027,11 @@
         </is>
       </c>
       <c r="I13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -986,28 +1051,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000064</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
         <v>64</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>3</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t xml:space="preserve"> Pardo / “Moreno” / Brown</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1027,20 +1097,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000121</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>121</v>
       </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F15" t="n">
+        <v>1</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1049,6 +1119,11 @@
         </is>
       </c>
       <c r="I15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1068,28 +1143,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000121</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>121</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>2</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1109,20 +1189,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000022</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>22</v>
       </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F17" t="n">
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1131,6 +1211,11 @@
         </is>
       </c>
       <c r="I17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1150,20 +1235,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000042</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
         <v>42</v>
       </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F18" t="n">
+        <v>1</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1172,6 +1257,11 @@
         </is>
       </c>
       <c r="I18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1191,20 +1281,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000085</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>85</v>
       </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F19" t="n">
+        <v>1</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1213,6 +1303,11 @@
         </is>
       </c>
       <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1232,20 +1327,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000044</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>44</v>
       </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F20" t="n">
+        <v>1</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1254,6 +1349,11 @@
         </is>
       </c>
       <c r="I20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1273,20 +1373,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000082</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>82</v>
       </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F21" t="n">
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1295,6 +1395,11 @@
         </is>
       </c>
       <c r="I21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1314,20 +1419,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000041</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>41</v>
       </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F22" t="n">
+        <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1336,6 +1441,11 @@
         </is>
       </c>
       <c r="I22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1355,20 +1465,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000067</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>67</v>
       </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F23" t="n">
+        <v>1</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1377,6 +1487,11 @@
         </is>
       </c>
       <c r="I23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1396,20 +1511,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000083</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
         <v>83</v>
       </c>
-      <c r="E24" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F24" t="n">
+        <v>1</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1418,6 +1533,11 @@
         </is>
       </c>
       <c r="I24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1437,20 +1557,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>1</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000001</t>
+        </is>
       </c>
       <c r="E25" t="n">
         <v>1</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F25" t="n">
+        <v>1</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1459,6 +1579,11 @@
         </is>
       </c>
       <c r="I25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1478,20 +1603,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000043</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
         <v>43</v>
       </c>
-      <c r="E26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F26" t="n">
+        <v>1</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1500,6 +1625,11 @@
         </is>
       </c>
       <c r="I26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1519,28 +1649,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000062</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>62</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>3</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t xml:space="preserve"> Pardo / “Moreno” / Brown</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H27" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1560,20 +1695,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000081</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>81</v>
       </c>
-      <c r="E28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F28" t="n">
+        <v>1</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1582,6 +1717,11 @@
         </is>
       </c>
       <c r="I28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1601,20 +1741,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000065</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>65</v>
       </c>
-      <c r="E29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F29" t="n">
+        <v>1</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1623,6 +1763,11 @@
         </is>
       </c>
       <c r="I29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1642,20 +1787,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000021</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
         <v>21</v>
       </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F30" t="n">
+        <v>1</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1664,6 +1809,11 @@
         </is>
       </c>
       <c r="I30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1683,20 +1833,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000084</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
         <v>84</v>
       </c>
-      <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F31" t="n">
+        <v>1</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1705,6 +1855,11 @@
         </is>
       </c>
       <c r="I31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1724,20 +1879,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000086</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
         <v>86</v>
       </c>
-      <c r="E32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F32" t="n">
+        <v>1</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1746,6 +1901,11 @@
         </is>
       </c>
       <c r="I32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1765,20 +1925,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000066</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
         <v>66</v>
       </c>
-      <c r="E33" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F33" t="n">
+        <v>1</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1787,6 +1947,11 @@
         </is>
       </c>
       <c r="I33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1806,20 +1971,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000061</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
         <v>61</v>
       </c>
-      <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F34" t="n">
+        <v>1</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1828,6 +1993,11 @@
         </is>
       </c>
       <c r="I34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1847,20 +2017,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000068</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
         <v>68</v>
       </c>
-      <c r="E35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F35" t="n">
+        <v>1</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1869,6 +2039,11 @@
         </is>
       </c>
       <c r="I35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1888,28 +2063,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D36" t="n">
-        <v>2</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000002</t>
+        </is>
       </c>
       <c r="E36" t="n">
         <v>2</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1929,20 +2109,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000063</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
         <v>63</v>
       </c>
-      <c r="E37" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F37" t="n">
+        <v>1</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1951,6 +2131,11 @@
         </is>
       </c>
       <c r="I37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -1970,20 +2155,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000123</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
         <v>123</v>
       </c>
-      <c r="E38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F38" t="n">
+        <v>1</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1992,6 +2177,11 @@
         </is>
       </c>
       <c r="I38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2011,28 +2201,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000064</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
         <v>64</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>2</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H39" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2052,28 +2247,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000121</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
         <v>121</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>3</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t xml:space="preserve"> Pardo / “Moreno” / Brown</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H40" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2093,20 +2293,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000022</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
         <v>22</v>
       </c>
-      <c r="E41" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F41" t="n">
+        <v>1</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2115,6 +2315,11 @@
         </is>
       </c>
       <c r="I41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2134,20 +2339,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000042</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
         <v>42</v>
       </c>
-      <c r="E42" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F42" t="n">
+        <v>1</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2156,6 +2361,11 @@
         </is>
       </c>
       <c r="I42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2175,20 +2385,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000085</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
         <v>85</v>
       </c>
-      <c r="E43" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F43" t="n">
+        <v>1</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2197,6 +2407,11 @@
         </is>
       </c>
       <c r="I43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2216,20 +2431,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000044</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
         <v>44</v>
       </c>
-      <c r="E44" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F44" t="n">
+        <v>1</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2238,6 +2453,11 @@
         </is>
       </c>
       <c r="I44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2257,20 +2477,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000082</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
         <v>82</v>
       </c>
-      <c r="E45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F45" t="n">
+        <v>1</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2279,6 +2499,11 @@
         </is>
       </c>
       <c r="I45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2298,20 +2523,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000041</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
         <v>41</v>
       </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F46" t="n">
+        <v>1</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2320,6 +2545,11 @@
         </is>
       </c>
       <c r="I46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2339,20 +2569,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000067</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
         <v>67</v>
       </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F47" t="n">
+        <v>1</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2361,6 +2591,11 @@
         </is>
       </c>
       <c r="I47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2380,20 +2615,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000083</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
         <v>83</v>
       </c>
-      <c r="E48" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F48" t="n">
+        <v>1</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2402,6 +2637,11 @@
         </is>
       </c>
       <c r="I48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2421,20 +2661,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>1</v>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000001</t>
+        </is>
       </c>
       <c r="E49" t="n">
         <v>1</v>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F49" t="n">
+        <v>1</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2443,6 +2683,11 @@
         </is>
       </c>
       <c r="I49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2462,20 +2707,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000043</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
         <v>43</v>
       </c>
-      <c r="E50" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F50" t="n">
+        <v>1</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2484,6 +2729,11 @@
         </is>
       </c>
       <c r="I50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2503,28 +2753,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000062</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
         <v>62</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>2</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H51" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2544,20 +2799,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D52" t="n">
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000081</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
         <v>81</v>
       </c>
-      <c r="E52" t="n">
-        <v>1</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F52" t="n">
+        <v>1</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2566,6 +2821,11 @@
         </is>
       </c>
       <c r="I52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2585,20 +2845,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000065</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
         <v>65</v>
       </c>
-      <c r="E53" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F53" t="n">
+        <v>1</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2607,6 +2867,11 @@
         </is>
       </c>
       <c r="I53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2626,20 +2891,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000021</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
         <v>21</v>
       </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F54" t="n">
+        <v>1</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2648,6 +2913,11 @@
         </is>
       </c>
       <c r="I54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2667,20 +2937,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000084</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
         <v>84</v>
       </c>
-      <c r="E55" t="n">
-        <v>1</v>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F55" t="n">
+        <v>1</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2689,6 +2959,11 @@
         </is>
       </c>
       <c r="I55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2708,20 +2983,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000086</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
         <v>86</v>
       </c>
-      <c r="E56" t="n">
-        <v>1</v>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F56" t="n">
+        <v>1</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2730,6 +3005,11 @@
         </is>
       </c>
       <c r="I56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2749,20 +3029,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D57" t="n">
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000066</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
         <v>66</v>
       </c>
-      <c r="E57" t="n">
-        <v>1</v>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F57" t="n">
+        <v>1</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2771,6 +3051,11 @@
         </is>
       </c>
       <c r="I57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2790,20 +3075,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000061</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
         <v>61</v>
       </c>
-      <c r="E58" t="n">
-        <v>1</v>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F58" t="n">
+        <v>1</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2812,6 +3097,11 @@
         </is>
       </c>
       <c r="I58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2831,20 +3121,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D59" t="n">
+      <c r="D59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000068</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
         <v>68</v>
       </c>
-      <c r="E59" t="n">
-        <v>1</v>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F59" t="n">
+        <v>1</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2853,6 +3143,11 @@
         </is>
       </c>
       <c r="I59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2872,28 +3167,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>2</v>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000002</t>
+        </is>
       </c>
       <c r="E60" t="n">
         <v>2</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H60" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2913,20 +3213,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D61" t="n">
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000063</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
         <v>63</v>
       </c>
-      <c r="E61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F61" t="n">
+        <v>1</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2935,6 +3235,11 @@
         </is>
       </c>
       <c r="I61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2954,20 +3259,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D62" t="n">
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000123</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
         <v>123</v>
       </c>
-      <c r="E62" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F62" t="n">
+        <v>1</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -2976,6 +3281,11 @@
         </is>
       </c>
       <c r="I62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -2995,28 +3305,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D63" t="n">
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000064</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
         <v>64</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>2</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="G63" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H63" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3036,28 +3351,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D64" t="n">
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000121</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
         <v>121</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>2</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="G64" t="inlineStr">
         <is>
           <t xml:space="preserve"> Preto / Negro / Black</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="H64" t="inlineStr">
         <is>
           <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3077,20 +3397,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D65" t="n">
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000022</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
         <v>22</v>
       </c>
-      <c r="E65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F65" t="n">
+        <v>1</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3099,6 +3419,11 @@
         </is>
       </c>
       <c r="I65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3118,20 +3443,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D66" t="n">
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000042</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
         <v>42</v>
       </c>
-      <c r="E66" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F66" t="n">
+        <v>1</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3140,6 +3465,11 @@
         </is>
       </c>
       <c r="I66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3159,20 +3489,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D67" t="n">
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000085</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
         <v>85</v>
       </c>
-      <c r="E67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F67" t="n">
+        <v>1</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -3181,6 +3511,11 @@
         </is>
       </c>
       <c r="I67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3200,20 +3535,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D68" t="n">
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000044</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
         <v>44</v>
       </c>
-      <c r="E68" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F68" t="n">
+        <v>1</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -3222,6 +3557,11 @@
         </is>
       </c>
       <c r="I68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3241,20 +3581,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000082</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
         <v>82</v>
       </c>
-      <c r="E69" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F69" t="n">
+        <v>1</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3263,6 +3603,11 @@
         </is>
       </c>
       <c r="I69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3282,20 +3627,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D70" t="n">
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000041</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
         <v>41</v>
       </c>
-      <c r="E70" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F70" t="n">
+        <v>1</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3304,6 +3649,11 @@
         </is>
       </c>
       <c r="I70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3323,20 +3673,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D71" t="n">
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000067</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
         <v>67</v>
       </c>
-      <c r="E71" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F71" t="n">
+        <v>1</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3345,6 +3695,11 @@
         </is>
       </c>
       <c r="I71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3364,20 +3719,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D72" t="n">
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000083</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
         <v>83</v>
       </c>
-      <c r="E72" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F72" t="n">
+        <v>1</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3386,6 +3741,11 @@
         </is>
       </c>
       <c r="I72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3405,20 +3765,20 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>1</v>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000001</t>
+        </is>
       </c>
       <c r="E73" t="n">
         <v>1</v>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Branco / Blanco / White</t>
-        </is>
+      <c r="F73" t="n">
+        <v>1</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> Branco / Blanco / White</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3427,6 +3787,11 @@
         </is>
       </c>
       <c r="I73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
         <is>
           <t>BR</t>
         </is>
@@ -3446,28 +3811,33 @@
           <t xml:space="preserve"> Candidatos Brasil 2014 (Candidaturas Majoritárias)</t>
         </is>
       </c>
-      <c r="D74" t="n">
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> foto_cand2014_div/FBR280000000043</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
         <v>43</v>
       </c>
-      <c r="E74" t="n">
+      <c r="F74" t="n">
         <v>3</v>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="G74" t="inlineStr">
         <is>
           <t xml:space="preserve"> Pardo / “Moreno” / Brown</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="H74" t="inlineStr">
         <is>
           <t xml:space="preserve"> S</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
       <c r="I74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
         <is>
           <t>BR</t>
         </is>

</xml_diff>